<commit_message>
black history month work continued
</commit_message>
<xml_diff>
--- a/data/black_history_month_data.xlsx
+++ b/data/black_history_month_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SChildress\Documents\GitHub\heritage-month\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DFD8F5-E275-4696-ADDC-AE734C207509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA612DA2-7747-4A53-BED9-4A64FCD4CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6BF6366D-BBDF-40F5-8D39-4EF720CAF928}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BF6366D-BBDF-40F5-8D39-4EF720CAF928}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pop by County 2010 2020" sheetId="1" r:id="rId1"/>
-    <sheet name="Racial Identity" sheetId="3" r:id="rId2"/>
+    <sheet name="Median income" sheetId="4" r:id="rId1"/>
+    <sheet name="Pop by County 2010 2020" sheetId="1" r:id="rId2"/>
+    <sheet name="Racial Identity" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Pop by County 2010 2020'!$A$4:$A$7</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>Region</t>
   </si>
@@ -107,6 +108,18 @@
   </si>
   <si>
     <t>Black Population Share</t>
+  </si>
+  <si>
+    <t>King County</t>
+  </si>
+  <si>
+    <t>Kitsap County</t>
+  </si>
+  <si>
+    <t>Pierce County</t>
+  </si>
+  <si>
+    <t>Snohomish County</t>
   </si>
   <si>
     <t>Black or African American alone</t>
@@ -180,12 +193,83 @@
   <si>
     <t>2020 People's Racial Identities who Identify as Black Alone or In Combination</t>
   </si>
+  <si>
+    <t>Note: Code for this work is on Github at: https://github.com/psrc/heritage-month</t>
+  </si>
+  <si>
+    <t>White, Non-Hispanic Householder Median Income</t>
+  </si>
+  <si>
+    <t>White, Non-Hispanic Householder Median Income MOE</t>
+  </si>
+  <si>
+    <t>Black Householder Median Income</t>
+  </si>
+  <si>
+    <r>
+      <t>Median Income by Black and White householders, ACS table 19013 (B, H), 2019 1-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>estimate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Median Income by Black and White householders, ACS table 19013 (B, H), 2019 5 -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>estimate</t>
+    </r>
+  </si>
+  <si>
+    <t>I'd go with 5-year estimate because of the wide error bars on the 1-year estimate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +291,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -269,6 +361,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -277,6 +389,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -341,63 +466,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,6 +548,1082 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Median Income by Black and White householders, ACS table 19013 (B, H), 2019 5 year estimate</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Median income'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Black Householder Median Income</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Median income'!$C$14:$C$17</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>2006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8640</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2765</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4023</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Median income'!$C$14:$C$17</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>2006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8640</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2765</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4023</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Median income'!$A$14:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Median income'!$B$14:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>49846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47074</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54683</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F797-4D71-98A7-16F135FF622E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Median income'!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>White, Non-Hispanic Householder Median Income</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Median income'!$E$14:$E$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>816</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1241</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1030</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1222</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Median income'!$E$14:$E$17</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>816</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1241</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1030</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1222</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Median income'!$A$14:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Median income'!$D$14:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>101265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77807</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F797-4D71-98A7-16F135FF622E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="173715248"/>
+        <c:axId val="173716912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="173715248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173716912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173716912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173715248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Median Income by Black and White householders, ACS table 19013 (B, H), 2019 1-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>year estimate</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Median income'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Black Householder Median Income</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Median income'!$C$3:$C$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5257</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19532</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>12325</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>19660</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Median income'!$C$3:$C$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5257</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19532</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>12325</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>19660</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Median income'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King County</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap County</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce County</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish County</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Median income'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>52462</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67143</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61188</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C20B-4728-80FD-C932D06DED73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Median income'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>White, Non-Hispanic Householder Median Income</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Median income'!$E$3:$E$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>2900</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4099</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2468</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3171</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Median income'!$E$3:$E$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>2900</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4099</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2468</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3171</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Median income'!$A$3:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>King County</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kitsap County</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pierce County</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Snohomish County</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Median income'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>109124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C20B-4728-80FD-C932D06DED73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="173715248"/>
+        <c:axId val="173716912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="173715248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173716912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173716912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173715248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -849,7 +2060,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1280,7 +2491,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1602,7 +2813,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2365,6 +3576,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3875,7 +5166,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3886,7 +5177,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3909,7 +5200,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -3932,16 +5223,19 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -3966,51 +5260,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -4025,8 +5304,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -4034,12 +5315,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -4049,13 +5327,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4074,16 +5352,18 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -4154,6 +5434,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -4185,8 +5471,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4241,7 +5527,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -4269,18 +5555,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -4290,9 +5565,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -4308,7 +5586,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4324,7 +5602,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4338,7 +5616,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -4371,7 +5649,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -4380,12 +5658,18 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4396,19 +5680,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1">
-          <a:lumMod val="65000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -4431,7 +5703,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -4454,16 +5726,19 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -4488,51 +5763,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -4547,8 +5807,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -4556,12 +5818,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -4571,13 +5830,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4596,16 +5855,18 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -4676,6 +5937,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -4707,8 +5974,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4763,7 +6030,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -4791,18 +6058,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -4812,9 +6068,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -4830,7 +6089,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4846,7 +6105,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4860,7 +6119,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -4893,7 +6152,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -4902,12 +6161,18 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4918,18 +6183,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1">
-          <a:lumMod val="65000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900"/>
   </cs:axisTitle>
   <cs:categoryAxis>
@@ -5428,7 +6681,1130 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>20637</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09FE99BD-799C-4099-8792-BF2C5E16B8BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>569913</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>568325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B51BBC-C738-4D5C-9E4A-C7C7919E9C41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5621,7 +7997,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6036,11 +8412,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA4F99D-F11C-4B51-BBC9-8709368647B0}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="18.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="32">
+        <v>52462</v>
+      </c>
+      <c r="C3" s="32">
+        <v>5257</v>
+      </c>
+      <c r="D3" s="32">
+        <v>109124</v>
+      </c>
+      <c r="E3" s="33">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="32">
+        <v>67143</v>
+      </c>
+      <c r="C4" s="32">
+        <v>19532</v>
+      </c>
+      <c r="D4" s="32">
+        <v>81317</v>
+      </c>
+      <c r="E4" s="33">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="32">
+        <v>61188</v>
+      </c>
+      <c r="C5" s="32">
+        <v>12325</v>
+      </c>
+      <c r="D5" s="32">
+        <v>83992</v>
+      </c>
+      <c r="E5" s="33">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="34">
+        <v>70107</v>
+      </c>
+      <c r="C6" s="34">
+        <v>19660</v>
+      </c>
+      <c r="D6" s="34">
+        <v>88946</v>
+      </c>
+      <c r="E6" s="35">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="32">
+        <v>49846</v>
+      </c>
+      <c r="C14" s="32">
+        <v>2006</v>
+      </c>
+      <c r="D14" s="32">
+        <v>101265</v>
+      </c>
+      <c r="E14" s="33">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="32">
+        <v>47074</v>
+      </c>
+      <c r="C15" s="32">
+        <v>8640</v>
+      </c>
+      <c r="D15" s="32">
+        <v>77807</v>
+      </c>
+      <c r="E15" s="33">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="32">
+        <v>54683</v>
+      </c>
+      <c r="C16" s="32">
+        <v>2765</v>
+      </c>
+      <c r="D16" s="32">
+        <v>76183</v>
+      </c>
+      <c r="E16" s="33">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="34">
+        <v>71050</v>
+      </c>
+      <c r="C17" s="34">
+        <v>4023</v>
+      </c>
+      <c r="D17" s="34">
+        <v>88341</v>
+      </c>
+      <c r="E17" s="35">
+        <v>1222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DD74AC-7B14-4C8A-84E8-6059B75DB471}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6049,169 +8629,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="29" t="s">
-        <v>42</v>
+      <c r="B1" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2"/>
-      <c r="B2" s="11">
+      <c r="A2" s="3"/>
+      <c r="B2" s="13">
         <v>2010</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14">
         <v>2020</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>147950</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>1931249</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <f>B4/C4</f>
         <v>7.6608453907290056E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>194857</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>2269675</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <f>E4/F4</f>
         <v>8.585237974599888E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>10086</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>251133</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <f t="shared" ref="D5:D8" si="0">B5/C5</f>
         <v>4.0161985879991875E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>13432</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>275611</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <f t="shared" ref="G5:G7" si="1">E5/F5</f>
         <v>4.873535526521075E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>74797</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>795225</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>9.4057656638058415E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>97967</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>921130</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <f t="shared" si="1"/>
         <v>0.10635523758861398</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>26069</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>713335</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>3.6545241716724963E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>43299</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>827957</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <f t="shared" si="1"/>
         <v>5.2296194126023453E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="20">
         <v>258902</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="21">
         <v>3690942</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="22">
         <f t="shared" si="0"/>
         <v>7.0145236636067435E-2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="20">
         <f>SUM(E4:E7)</f>
         <v>349555</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="21">
         <f>SUM(F4:F7)</f>
         <v>4294373</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="22">
         <f>E8/F8</f>
         <v>8.139837876216155E-2</v>
       </c>
@@ -6230,139 +8810,144 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="29" t="s">
-        <v>43</v>
+      <c r="B11" s="31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <f>E4-B4</f>
         <v>46907</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <f>B14/B4</f>
         <v>0.31704629942548157</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="17">
         <f>F4-C4</f>
         <v>338426</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <f>D14/C4</f>
         <v>0.17523685449157514</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <f>E5-B5</f>
         <v>3346</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <f>B15/B5</f>
         <v>0.33174697600634545</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="17">
         <f>F5-C5</f>
         <v>24478</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <f>D15/C5</f>
         <v>9.74702647601072E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <f>E6-B6</f>
         <v>23170</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <f>B16/B6</f>
         <v>0.3097717822907336</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="17">
         <f>F6-C6</f>
         <v>125905</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="7">
         <f>D16/C6</f>
         <v>0.15832625986356064</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <f>E7-B7</f>
         <v>17230</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <f>B17/B7</f>
         <v>0.66093827918217041</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="17">
         <f>F7-C7</f>
         <v>114622</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="7">
         <f>D17/C7</f>
         <v>0.16068467129749697</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="20">
         <f>E8-B8</f>
         <v>90653</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="23">
         <f>B18/B8</f>
         <v>0.35014406995697211</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="24">
         <f>F8-C8</f>
         <v>603431</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="22">
         <f>D18/C8</f>
         <v>0.16348969991942436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -6382,12 +8967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9888BC98-F078-48BD-A3BD-24A6E80C418D}">
-  <dimension ref="A1:AS31"/>
+  <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6398,118 +8983,118 @@
     <row r="1" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="W2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="X2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="Y2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="Z2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AB2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AC2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AD2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AE2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AF2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AG2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AH2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AI2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AJ2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AK2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AL2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AM2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AN2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AO2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AP2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AQ2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AR2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AS2" t="s">
         <v>3</v>
@@ -6517,18 +9102,18 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G3">
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>33</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="K3">
@@ -6637,18 +9222,18 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>35</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K4">
@@ -6757,18 +9342,18 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G5">
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I5">
         <v>53</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K5">
@@ -6877,21 +9462,21 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G6">
         <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>61</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="K6">
@@ -6999,8 +9584,8 @@
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="J7" s="23" t="s">
-        <v>36</v>
+      <c r="J7" s="25" t="s">
+        <v>40</v>
       </c>
       <c r="K7">
         <f>SUM(K3:K6)</f>
@@ -7136,98 +9721,98 @@
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="C15" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="C15" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="25" t="s">
+      <c r="J16" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="K16" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>41</v>
+      </c>
       <c r="M16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="25">
+      <c r="B17" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="27">
         <f>K7</f>
         <v>254602</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="27">
         <f t="shared" ref="D17:L17" si="2">L7</f>
         <v>54283</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="27">
         <f t="shared" si="2"/>
         <v>4755</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="27">
         <f t="shared" si="2"/>
         <v>7297</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="27">
         <f t="shared" si="2"/>
         <v>1756</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="27">
         <f t="shared" si="2"/>
         <v>5529</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="27">
         <f t="shared" si="2"/>
         <v>7219</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="27">
         <f t="shared" si="2"/>
         <v>5102</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="27">
         <f t="shared" si="2"/>
         <v>3099</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="27">
         <f t="shared" si="2"/>
         <v>5913</v>
       </c>
@@ -7237,69 +9822,69 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="27">
+      <c r="B18" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="29">
         <f>C17/$M$17</f>
         <v>0.7283603438657722</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="29">
         <f t="shared" ref="D18:L18" si="3">D17/$M$17</f>
         <v>0.15529172805424038</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="29">
         <f t="shared" si="3"/>
         <v>1.360300954070175E-2</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="29">
         <f t="shared" si="3"/>
         <v>2.0875112643217807E-2</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="29">
         <f t="shared" si="3"/>
         <v>5.0235299166082594E-3</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="29">
         <f t="shared" si="3"/>
         <v>1.5817253364992633E-2</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="29">
         <f t="shared" si="3"/>
         <v>2.065197179270787E-2</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18" s="29">
         <f t="shared" si="3"/>
         <v>1.4595700247457481E-2</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="29">
         <f t="shared" si="3"/>
         <v>8.8655576375677655E-3</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="29">
         <f t="shared" si="3"/>
         <v>1.6915792936733846E-2</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>254602</v>
@@ -7310,7 +9895,7 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D23">
         <v>54283</v>
@@ -7321,7 +9906,7 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <v>4755</v>
@@ -7332,7 +9917,7 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D25">
         <v>7297</v>
@@ -7343,7 +9928,7 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D26">
         <v>1756</v>
@@ -7354,7 +9939,7 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>5529</v>
@@ -7365,7 +9950,7 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D28">
         <v>7219</v>
@@ -7376,7 +9961,7 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D29">
         <v>5102</v>
@@ -7387,7 +9972,7 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D30">
         <v>3099</v>
@@ -7398,13 +9983,18 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D31">
         <v>5913</v>
       </c>
       <c r="E31" s="1">
         <v>1.6915792936733846E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for black history month data
</commit_message>
<xml_diff>
--- a/data/black_history_month_data.xlsx
+++ b/data/black_history_month_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SChildress\Documents\GitHub\heritage-month\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F89646-C872-4E83-A2D3-2CC887EB07DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48B6AD-5709-49C9-8754-654892BCB01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="7" activeTab="12" xr2:uid="{6BF6366D-BBDF-40F5-8D39-4EF720CAF928}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BF6366D-BBDF-40F5-8D39-4EF720CAF928}"/>
   </bookViews>
   <sheets>
     <sheet name="Median income" sheetId="4" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="TransporttoWork" sheetId="6" r:id="rId12"/>
     <sheet name="Map" sheetId="10" r:id="rId13"/>
     <sheet name="WomenGaveBirth" sheetId="13" r:id="rId14"/>
+    <sheet name="travelsurveynotes" sheetId="17" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Pop by County 2010 2020'!$A$4:$A$7</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="212">
   <si>
     <t>Region</t>
   </si>
@@ -725,6 +726,18 @@
   </si>
   <si>
     <t>health insurance</t>
+  </si>
+  <si>
+    <t>One in five Black/African American households in the region have no cars. By comparison, one in 20 white households (5%) are car-less. Asians, Hispanics, and people of other races were slightly more likely than white households to be without cars (7%). Because people of color had fewer cars, they were significantly more likely to use transit than whites. While 16% of African Americans used transit five or more days a week, only 6% of whites rode transit this often. On any given trip, Black survey participants were four times as likely as whites to use a bus or train. They used this mode for about 12% of their trips, while only 4% of whites used public transportation. Asians chose transit for 8% of their trips, while Hispanics and people of other races used this mode 5% of the time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOE </t>
+  </si>
+  <si>
+    <t>Black Adults (total)</t>
+  </si>
+  <si>
+    <t>White Adults (total)</t>
   </si>
 </sst>
 </file>
@@ -1167,11 +1180,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14543,8 +14556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA4F99D-F11C-4B51-BBC9-8709368647B0}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15055,10 +15068,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="82"/>
+      <c r="C1" s="81"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -15494,7 +15507,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="40"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="74"/>
@@ -15733,7 +15746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E92C88B-E51A-4891-86D1-5015B4F1E45E}">
   <dimension ref="D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -15958,6 +15971,26 @@
       <c r="O6" s="72">
         <f>O4/O3</f>
         <v>4.8346604015237583E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C1A047-89E3-46DF-8CB8-646C6E8E392B}">
+  <dimension ref="B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -16271,16 +16304,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00ABD136-B943-4560-9FDA-7DAF09475023}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.36328125" customWidth="1"/>
-    <col min="2" max="3" width="7.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" customWidth="1"/>
+    <col min="3" max="3" width="35.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
@@ -16315,11 +16349,11 @@
         <v>90</v>
       </c>
       <c r="B4" s="46">
-        <f>(A23+A18)/A$16</f>
+        <f>(D22+D17)/D$15</f>
         <v>0.255785749032099</v>
       </c>
       <c r="C4" s="47">
-        <f>(D23+D18)/D$16</f>
+        <f>(B22+B17)/B$15</f>
         <v>0.4398081805246033</v>
       </c>
       <c r="D4" s="51"/>
@@ -16332,11 +16366,11 @@
         <v>91</v>
       </c>
       <c r="B5" s="46">
-        <f>(A24+A19)/A$16</f>
+        <f>(D23+D18)/D$15</f>
         <v>0.25610560616258071</v>
       </c>
       <c r="C5" s="47">
-        <f>(D24+D19)/D$16</f>
+        <f>(B23+B18)/B$15</f>
         <v>0.19509283325461699</v>
       </c>
       <c r="D5" s="51"/>
@@ -16349,11 +16383,11 @@
         <v>92</v>
       </c>
       <c r="B6" s="46">
-        <f>(A25+A20)/A$16</f>
+        <f>(D24+D19)/D$15</f>
         <v>0.10234095437371307</v>
       </c>
       <c r="C6" s="47">
-        <f>(D25+D20)/D$16</f>
+        <f>(B24+B19)/B$15</f>
         <v>4.1312485083336944E-2</v>
       </c>
       <c r="D6" s="51"/>
@@ -16366,11 +16400,11 @@
         <v>93</v>
       </c>
       <c r="B7" s="49">
-        <f>(A26+A21)/A$16</f>
+        <f>(D25+D20)/D$15</f>
         <v>0.38576769043160719</v>
       </c>
       <c r="C7" s="50">
-        <f>(D26+D21)/D$16</f>
+        <f>(B25+B20)/B$15</f>
         <v>0.32378650113744278</v>
       </c>
       <c r="D7" s="51"/>
@@ -16417,211 +16451,206 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>1986034</v>
+      </c>
+      <c r="C15">
+        <v>643.40267329255005</v>
+      </c>
+      <c r="D15">
+        <v>150067</v>
+      </c>
+      <c r="E15">
+        <v>1497.47621016162</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>150067</v>
+      <c r="A16" t="s">
+        <v>80</v>
       </c>
       <c r="B16">
-        <v>1497.47621016162</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
+        <v>998515</v>
+      </c>
+      <c r="C16">
+        <v>358.36294451296197</v>
       </c>
       <c r="D16">
-        <v>1986034</v>
+        <v>70031</v>
       </c>
       <c r="E16">
-        <v>643.40267329255005</v>
+        <v>927.74457691759096</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>70031</v>
+      <c r="A17" t="s">
+        <v>81</v>
       </c>
       <c r="B17">
-        <v>927.74457691759096</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
+        <v>436959</v>
+      </c>
+      <c r="C17">
+        <v>2937.7830076436899</v>
       </c>
       <c r="D17">
-        <v>998515</v>
+        <v>17256</v>
       </c>
       <c r="E17">
-        <v>358.36294451296197</v>
+        <v>968.26287752861799</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17256</v>
+      <c r="A18" t="s">
+        <v>82</v>
       </c>
       <c r="B18">
-        <v>968.26287752861799</v>
-      </c>
-      <c r="C18" t="s">
-        <v>81</v>
+        <v>189505</v>
+      </c>
+      <c r="C18">
+        <v>2568.75553527384</v>
       </c>
       <c r="D18">
-        <v>436959</v>
+        <v>17068</v>
       </c>
       <c r="E18">
-        <v>2937.7830076436899</v>
+        <v>1046.6350844492099</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>17068</v>
+      <c r="A19" t="s">
+        <v>83</v>
       </c>
       <c r="B19">
-        <v>1046.6350844492099</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
+        <v>37781</v>
+      </c>
+      <c r="C19">
+        <v>1357.7227257433699</v>
       </c>
       <c r="D19">
-        <v>189505</v>
+        <v>8658</v>
       </c>
       <c r="E19">
-        <v>2568.75553527384</v>
+        <v>658.71541654951398</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>8658</v>
+      <c r="A20" t="s">
+        <v>84</v>
       </c>
       <c r="B20">
-        <v>658.71541654951398</v>
-      </c>
-      <c r="C20" t="s">
-        <v>83</v>
+        <v>334270</v>
+      </c>
+      <c r="C20">
+        <v>3207.7962840554601</v>
       </c>
       <c r="D20">
-        <v>37781</v>
+        <v>27049</v>
       </c>
       <c r="E20">
-        <v>1357.7227257433699</v>
+        <v>1134.1895785096999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>27049</v>
+      <c r="A21" t="s">
+        <v>85</v>
       </c>
       <c r="B21">
-        <v>1134.1895785096999</v>
-      </c>
-      <c r="C21" t="s">
-        <v>84</v>
+        <v>987519</v>
+      </c>
+      <c r="C21">
+        <v>395.02025264535501</v>
       </c>
       <c r="D21">
-        <v>334270</v>
+        <v>80036</v>
       </c>
       <c r="E21">
-        <v>3207.7962840554601</v>
+        <v>984.92436257816303</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>80036</v>
+      <c r="A22" t="s">
+        <v>86</v>
       </c>
       <c r="B22">
-        <v>984.92436257816303</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
+        <v>436515</v>
+      </c>
+      <c r="C22">
+        <v>3329.6273064714001</v>
       </c>
       <c r="D22">
-        <v>987519</v>
+        <v>21129</v>
       </c>
       <c r="E22">
-        <v>395.02025264535501</v>
+        <v>1043.2583572634301</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>21129</v>
+      <c r="A23" t="s">
+        <v>87</v>
       </c>
       <c r="B23">
-        <v>1043.2583572634301</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
+        <v>197956</v>
+      </c>
+      <c r="C23">
+        <v>3021.8097226661998</v>
       </c>
       <c r="D23">
-        <v>436515</v>
+        <v>21365</v>
       </c>
       <c r="E23">
-        <v>3329.6273064714001</v>
+        <v>1277.50107632049</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>21365</v>
+      <c r="A24" t="s">
+        <v>88</v>
       </c>
       <c r="B24">
-        <v>1277.50107632049</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
+        <v>44267</v>
+      </c>
+      <c r="C24">
+        <v>1435.1870958171301</v>
       </c>
       <c r="D24">
-        <v>197956</v>
+        <v>6700</v>
       </c>
       <c r="E24">
-        <v>3021.8097226661998</v>
+        <v>699.04291713742396</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>6700</v>
+      <c r="A25" t="s">
+        <v>89</v>
       </c>
       <c r="B25">
-        <v>699.04291713742396</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
+        <v>308781</v>
+      </c>
+      <c r="C25">
+        <v>3219.5437564971799</v>
       </c>
       <c r="D25">
-        <v>44267</v>
+        <v>30842</v>
       </c>
       <c r="E25">
-        <v>1435.1870958171301</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>30842</v>
-      </c>
-      <c r="B26">
         <v>1241.2070737793899</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26">
-        <v>308781</v>
-      </c>
-      <c r="E26">
-        <v>3219.5437564971799</v>
       </c>
     </row>
   </sheetData>
@@ -16629,7 +16658,8 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18565,10 +18595,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="81"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -18650,10 +18680,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="80" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="81"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">

</xml_diff>